<commit_message>
add post, get, delete implementing with data driven test
</commit_message>
<xml_diff>
--- a/datatest/datatesting.xlsx
+++ b/datatest/datatesting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kazakimaru\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kazakimaru\IdeaProjects\API-Testing-Rest-Assured-Java\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28BC55B9-6DA8-4B20-89A1-F0460B09934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B347A18A-35F0-404C-BF9D-6183D68F8FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{164DB088-93D1-4B68-86FE-D35F88C98C8A}"/>
   </bookViews>
@@ -45,30 +45,6 @@
     <t>PHONE</t>
   </si>
   <si>
-    <t>1passawdjwa0</t>
-  </si>
-  <si>
-    <t>1passawdjwa1</t>
-  </si>
-  <si>
-    <t>1passawdjwa2</t>
-  </si>
-  <si>
-    <t>1passawdjwa3</t>
-  </si>
-  <si>
-    <t>deoanwadaw-d1</t>
-  </si>
-  <si>
-    <t>deoanwadaw-d2</t>
-  </si>
-  <si>
-    <t>deoanwadaw-d3</t>
-  </si>
-  <si>
-    <t>deoanwadaw-d4</t>
-  </si>
-  <si>
     <t>1mail1@mail.com</t>
   </si>
   <si>
@@ -81,28 +57,52 @@
     <t>4mail1@mail.com</t>
   </si>
   <si>
-    <t>aowdjapodja1</t>
-  </si>
-  <si>
-    <t>aowdjapodja2</t>
-  </si>
-  <si>
-    <t>aowdjapodja3</t>
-  </si>
-  <si>
-    <t>aowdjapodja4</t>
-  </si>
-  <si>
-    <t>belajangiawi0ad1</t>
-  </si>
-  <si>
-    <t>belajangiawi0ad2</t>
-  </si>
-  <si>
-    <t>belajangiawi0ad3</t>
-  </si>
-  <si>
-    <t>belajangiawi0ad4</t>
+    <t>uname1</t>
+  </si>
+  <si>
+    <t>uname2</t>
+  </si>
+  <si>
+    <t>uname3</t>
+  </si>
+  <si>
+    <t>uname4</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>password3</t>
+  </si>
+  <si>
+    <t>password4</t>
+  </si>
+  <si>
+    <t>lastname1</t>
+  </si>
+  <si>
+    <t>lastname2</t>
+  </si>
+  <si>
+    <t>lastname3</t>
+  </si>
+  <si>
+    <t>lastname4</t>
+  </si>
+  <si>
+    <t>firstname1</t>
+  </si>
+  <si>
+    <t>firstname2</t>
+  </si>
+  <si>
+    <t>firstname3</t>
+  </si>
+  <si>
+    <t>firstname4</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,16 +509,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -529,16 +529,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -549,16 +549,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -569,16 +569,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>

</xml_diff>